<commit_message>
data actualizada por region
</commit_message>
<xml_diff>
--- a/data/2020/2020-03-18/covid19peru.xlsx
+++ b/data/2020/2020-03-18/covid19peru.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABCN\Github\manos-a-la-data\data\2020\2020-03-18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE50A962-B7B8-4D37-B0FA-A1FF708EB2BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED9E114-ADB7-40EA-BCC5-FFB50A53E268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>dia</t>
   </si>
@@ -49,6 +50,42 @@
   </si>
   <si>
     <t>muertos</t>
+  </si>
+  <si>
+    <t>Lima</t>
+  </si>
+  <si>
+    <t>Loreto</t>
+  </si>
+  <si>
+    <t>Lambayeque</t>
+  </si>
+  <si>
+    <t>Callao</t>
+  </si>
+  <si>
+    <t>Cusco</t>
+  </si>
+  <si>
+    <t>Ancash</t>
+  </si>
+  <si>
+    <t>Arequipa</t>
+  </si>
+  <si>
+    <t>La Libertad</t>
+  </si>
+  <si>
+    <t>Piura</t>
+  </si>
+  <si>
+    <t>Ica</t>
+  </si>
+  <si>
+    <t>Madre de Dios</t>
+  </si>
+  <si>
+    <t>Huanuco</t>
   </si>
 </sst>
 </file>
@@ -72,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,6 +119,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -98,13 +141,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,6 +443,648 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>43896</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>43897</v>
+      </c>
+      <c r="B3" s="1">
+        <f>B2+1</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D15" si="0">C3-C2</f>
+        <v>5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>43898</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:B15" si="1">B3+1</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>43899</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>43900</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>43901</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>43902</v>
+      </c>
+      <c r="B8" s="8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="8">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>43903</v>
+      </c>
+      <c r="B9" s="8">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="8">
+        <v>38</v>
+      </c>
+      <c r="D9" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>32</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8">
+        <v>1</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8">
+        <v>2</v>
+      </c>
+      <c r="M9" s="8">
+        <v>2</v>
+      </c>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="8"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>43904</v>
+      </c>
+      <c r="B10" s="8">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="8">
+        <v>43</v>
+      </c>
+      <c r="D10" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>37</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8">
+        <v>1</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8">
+        <v>2</v>
+      </c>
+      <c r="M10" s="8">
+        <v>2</v>
+      </c>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>43905</v>
+      </c>
+      <c r="B11" s="8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="8">
+        <v>71</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8">
+        <v>58</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+      <c r="I11" s="8">
+        <v>2</v>
+      </c>
+      <c r="J11" s="8">
+        <v>1</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1</v>
+      </c>
+      <c r="L11" s="8">
+        <v>2</v>
+      </c>
+      <c r="M11" s="8">
+        <v>2</v>
+      </c>
+      <c r="N11" s="8">
+        <v>1</v>
+      </c>
+      <c r="O11" s="8">
+        <v>2</v>
+      </c>
+      <c r="P11" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="8"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>43906</v>
+      </c>
+      <c r="B12" s="8">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C12" s="8">
+        <v>86</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>70</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8">
+        <v>3</v>
+      </c>
+      <c r="I12" s="8">
+        <v>3</v>
+      </c>
+      <c r="J12" s="8">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8">
+        <v>2</v>
+      </c>
+      <c r="M12" s="8">
+        <v>2</v>
+      </c>
+      <c r="N12" s="8">
+        <v>1</v>
+      </c>
+      <c r="O12" s="8">
+        <v>2</v>
+      </c>
+      <c r="P12" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="8"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>43907</v>
+      </c>
+      <c r="B13" s="8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="8">
+        <v>117</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8">
+        <v>96</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8">
+        <v>6</v>
+      </c>
+      <c r="I13" s="8">
+        <v>4</v>
+      </c>
+      <c r="J13" s="8">
+        <v>1</v>
+      </c>
+      <c r="K13" s="8">
+        <v>1</v>
+      </c>
+      <c r="L13" s="8">
+        <v>2</v>
+      </c>
+      <c r="M13" s="8">
+        <v>2</v>
+      </c>
+      <c r="N13" s="8">
+        <v>1</v>
+      </c>
+      <c r="O13" s="8">
+        <v>2</v>
+      </c>
+      <c r="P13" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="8"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>43908</v>
+      </c>
+      <c r="B14" s="8">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C14" s="8">
+        <v>145</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8">
+        <v>111</v>
+      </c>
+      <c r="G14" s="8">
+        <v>10</v>
+      </c>
+      <c r="H14" s="8">
+        <v>6</v>
+      </c>
+      <c r="I14" s="8">
+        <v>5</v>
+      </c>
+      <c r="J14" s="8">
+        <v>1</v>
+      </c>
+      <c r="K14" s="8">
+        <v>2</v>
+      </c>
+      <c r="L14" s="8">
+        <v>2</v>
+      </c>
+      <c r="M14" s="8">
+        <v>2</v>
+      </c>
+      <c r="N14" s="8">
+        <v>2</v>
+      </c>
+      <c r="O14" s="8">
+        <v>2</v>
+      </c>
+      <c r="P14" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>43909</v>
+      </c>
+      <c r="B15" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="8">
+        <v>234</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="E15" s="8">
+        <v>3</v>
+      </c>
+      <c r="F15" s="8">
+        <v>194</v>
+      </c>
+      <c r="G15" s="8">
+        <v>11</v>
+      </c>
+      <c r="H15" s="8">
+        <v>6</v>
+      </c>
+      <c r="I15" s="8">
+        <v>5</v>
+      </c>
+      <c r="J15" s="8">
+        <v>4</v>
+      </c>
+      <c r="K15" s="8">
+        <v>3</v>
+      </c>
+      <c r="L15" s="8">
+        <v>3</v>
+      </c>
+      <c r="M15" s="8">
+        <v>2</v>
+      </c>
+      <c r="N15" s="8">
+        <v>2</v>
+      </c>
+      <c r="O15" s="8">
+        <v>2</v>
+      </c>
+      <c r="P15" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA75DE2-DFBF-4DD1-886E-7BF3BF81DB3E}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -444,7 +1144,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D11" si="0">C3-C2</f>
+        <f t="shared" ref="D3:D15" si="0">C3-C2</f>
         <v>5</v>
       </c>
       <c r="E3" s="1">
@@ -615,7 +1315,7 @@
         <v>86</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" ref="D12:D13" si="2">C12-C11</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E12" s="1">
@@ -634,7 +1334,7 @@
         <v>117</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="E13" s="1">
@@ -653,7 +1353,7 @@
         <v>145</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14" si="3">C14-C13</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="E14" s="1">
@@ -672,7 +1372,7 @@
         <v>234</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" ref="D15" si="4">C15-C14</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
       <c r="E15" s="1">
@@ -684,12 +1384,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D305DDB7-21EF-4064-9B3A-06591E83BC3A}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +1399,7 @@
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -715,8 +1415,44 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43896</v>
       </c>
@@ -733,7 +1469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43897</v>
       </c>
@@ -752,7 +1488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43898</v>
       </c>
@@ -771,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>43899</v>
       </c>
@@ -790,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>43900</v>
       </c>
@@ -809,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>43901</v>
       </c>
@@ -828,7 +1564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>43902</v>
       </c>
@@ -847,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>43903</v>
       </c>
@@ -865,8 +1601,23 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <v>32</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>43904</v>
       </c>
@@ -884,8 +1635,23 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
+        <v>37</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>43905</v>
       </c>
@@ -903,8 +1669,38 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <v>58</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>43906</v>
       </c>
@@ -922,8 +1718,38 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <v>70</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>43907</v>
       </c>
@@ -941,8 +1767,41 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>96</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>43908</v>
       </c>
@@ -960,8 +1819,44 @@
       <c r="E14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <v>111</v>
+      </c>
+      <c r="G14" s="1">
+        <v>10</v>
+      </c>
+      <c r="H14" s="1">
+        <v>6</v>
+      </c>
+      <c r="I14" s="1">
+        <v>5</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1">
+        <v>2</v>
+      </c>
+      <c r="L14" s="1">
+        <v>2</v>
+      </c>
+      <c r="M14" s="1">
+        <v>2</v>
+      </c>
+      <c r="N14" s="1">
+        <v>2</v>
+      </c>
+      <c r="O14" s="1">
+        <v>2</v>
+      </c>
+      <c r="P14" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>43909</v>
       </c>
@@ -978,6 +1873,42 @@
       </c>
       <c r="E15" s="1">
         <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>194</v>
+      </c>
+      <c r="G15" s="1">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1">
+        <v>6</v>
+      </c>
+      <c r="I15" s="1">
+        <v>5</v>
+      </c>
+      <c r="J15" s="1">
+        <v>4</v>
+      </c>
+      <c r="K15" s="1">
+        <v>3</v>
+      </c>
+      <c r="L15" s="1">
+        <v>3</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2</v>
+      </c>
+      <c r="N15" s="1">
+        <v>2</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizando hasta el 24
</commit_message>
<xml_diff>
--- a/data/2020/2020-03-18/covid19peru.xlsx
+++ b/data/2020/2020-03-18/covid19peru.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABCN\Github\manos-a-la-data\data\2020\2020-03-18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943B3676-C7B2-41AA-823F-31A49BB90DF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCE535C-6797-430F-AC79-D9C856ED196C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja7" sheetId="7" r:id="rId2"/>
-    <sheet name="distritos" sheetId="8" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId5"/>
-    <sheet name="Hoja4" sheetId="4" r:id="rId6"/>
-    <sheet name="edad" sheetId="6" r:id="rId7"/>
+    <sheet name="Hoja6" sheetId="10" r:id="rId2"/>
+    <sheet name="Hoja5" sheetId="9" r:id="rId3"/>
+    <sheet name="Hoja7" sheetId="7" r:id="rId4"/>
+    <sheet name="distritos" sheetId="8" r:id="rId5"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId6"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId7"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId8"/>
+    <sheet name="edad" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>dia</t>
   </si>
@@ -168,6 +170,12 @@
   </si>
   <si>
     <t>UCI</t>
+  </si>
+  <si>
+    <t>dia de emergencia</t>
+  </si>
+  <si>
+    <t>al medio dia</t>
   </si>
 </sst>
 </file>
@@ -229,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,6 +260,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,37 +834,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD19"/>
+  <dimension ref="A1:AE20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -861,107 +873,110 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43896</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -973,8 +988,9 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43897</v>
       </c>
@@ -982,17 +998,17 @@
         <f>B2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
-        <f t="shared" ref="D3:D15" si="0">C3-C2</f>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E15" si="0">D3-D2</f>
         <v>5</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1004,26 +1020,27 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43898</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B19" si="1">B3+1</f>
+        <f t="shared" ref="B4:B20" si="1">B3+1</f>
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
         <v>7</v>
       </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1035,8 +1052,9 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43899</v>
       </c>
@@ -1044,17 +1062,17 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
         <v>9</v>
       </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1"/>
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1066,8 +1084,9 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43900</v>
       </c>
@@ -1075,17 +1094,17 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
         <v>11</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1"/>
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1097,8 +1116,9 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43901</v>
       </c>
@@ -1106,17 +1126,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
         <v>17</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1128,8 +1148,9 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>43902</v>
       </c>
@@ -1137,17 +1158,17 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8">
         <v>22</v>
       </c>
-      <c r="D8" s="8">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -1159,8 +1180,9 @@
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R8" s="8"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>43903</v>
       </c>
@@ -1168,40 +1190,41 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8">
         <v>38</v>
       </c>
-      <c r="D9" s="8">
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
       <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
         <v>32</v>
       </c>
-      <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="8">
-        <v>1</v>
-      </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8">
-        <v>2</v>
-      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8">
+        <v>1</v>
+      </c>
+      <c r="L9" s="8"/>
       <c r="M9" s="8">
         <v>2</v>
       </c>
-      <c r="N9" s="8"/>
+      <c r="N9" s="8">
+        <v>2</v>
+      </c>
       <c r="O9" s="8"/>
-      <c r="P9" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="8"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8">
+        <v>1</v>
+      </c>
+      <c r="R9" s="8"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>43904</v>
       </c>
@@ -1209,40 +1232,41 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8">
         <v>43</v>
       </c>
-      <c r="D10" s="8">
+      <c r="E10" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E10" s="8">
-        <v>0</v>
-      </c>
       <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
         <v>37</v>
       </c>
-      <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="8">
-        <v>1</v>
-      </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8">
-        <v>2</v>
-      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8">
+        <v>1</v>
+      </c>
+      <c r="L10" s="8"/>
       <c r="M10" s="8">
         <v>2</v>
       </c>
-      <c r="N10" s="8"/>
+      <c r="N10" s="8">
+        <v>2</v>
+      </c>
       <c r="O10" s="8"/>
-      <c r="P10" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="8"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8">
+        <v>1</v>
+      </c>
+      <c r="R10" s="8"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>43905</v>
       </c>
@@ -1250,50 +1274,51 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8">
         <v>71</v>
       </c>
-      <c r="D11" s="8">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
       <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
         <v>58</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8">
-        <v>1</v>
-      </c>
+      <c r="H11" s="8"/>
       <c r="I11" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="8">
         <v>1</v>
       </c>
       <c r="L11" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M11" s="8">
         <v>2</v>
       </c>
       <c r="N11" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P11" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="8"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>1</v>
+      </c>
+      <c r="R11" s="8"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>43906</v>
       </c>
@@ -1302,49 +1327,52 @@
         <v>11</v>
       </c>
       <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8">
         <v>86</v>
       </c>
-      <c r="D12" s="8">
+      <c r="E12" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
       <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
         <v>70</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8">
-        <v>3</v>
-      </c>
+      <c r="H12" s="8"/>
       <c r="I12" s="8">
         <v>3</v>
       </c>
       <c r="J12" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K12" s="8">
         <v>1</v>
       </c>
       <c r="L12" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12" s="8">
         <v>2</v>
       </c>
       <c r="N12" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P12" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="8"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>1</v>
+      </c>
+      <c r="R12" s="8"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>43907</v>
       </c>
@@ -1353,51 +1381,54 @@
         <v>12</v>
       </c>
       <c r="C13" s="8">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8">
         <v>117</v>
       </c>
-      <c r="D13" s="8">
+      <c r="E13" s="8">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
       <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
         <v>96</v>
       </c>
-      <c r="G13" s="8">
-        <v>1</v>
-      </c>
       <c r="H13" s="8">
+        <v>1</v>
+      </c>
+      <c r="I13" s="8">
         <v>6</v>
       </c>
-      <c r="I13" s="8">
+      <c r="J13" s="8">
         <v>4</v>
       </c>
-      <c r="J13" s="8">
-        <v>1</v>
-      </c>
       <c r="K13" s="8">
         <v>1</v>
       </c>
       <c r="L13" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M13" s="8">
         <v>2</v>
       </c>
       <c r="N13" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P13" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="8"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>1</v>
+      </c>
+      <c r="R13" s="8"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>43908</v>
       </c>
@@ -1406,32 +1437,32 @@
         <v>13</v>
       </c>
       <c r="C14" s="8">
+        <v>3</v>
+      </c>
+      <c r="D14" s="8">
         <v>145</v>
       </c>
-      <c r="D14" s="8">
+      <c r="E14" s="8">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E14" s="8">
-        <v>0</v>
-      </c>
       <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
         <v>111</v>
       </c>
-      <c r="G14" s="8">
+      <c r="H14" s="8">
         <v>10</v>
       </c>
-      <c r="H14" s="8">
+      <c r="I14" s="8">
         <v>6</v>
       </c>
-      <c r="I14" s="8">
+      <c r="J14" s="8">
         <v>5</v>
       </c>
-      <c r="J14" s="8">
-        <v>1</v>
-      </c>
       <c r="K14" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L14" s="8">
         <v>2</v>
@@ -1446,13 +1477,16 @@
         <v>2</v>
       </c>
       <c r="P14" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>43909</v>
       </c>
@@ -1461,38 +1495,38 @@
         <v>14</v>
       </c>
       <c r="C15" s="8">
+        <v>4</v>
+      </c>
+      <c r="D15" s="8">
         <v>234</v>
       </c>
-      <c r="D15" s="8">
+      <c r="E15" s="8">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="E15" s="8">
+      <c r="F15" s="8">
         <v>3</v>
       </c>
-      <c r="F15" s="8">
+      <c r="G15" s="8">
         <v>194</v>
       </c>
-      <c r="G15" s="8">
+      <c r="H15" s="8">
         <v>11</v>
       </c>
-      <c r="H15" s="8">
+      <c r="I15" s="8">
         <v>6</v>
       </c>
-      <c r="I15" s="8">
+      <c r="J15" s="8">
         <v>5</v>
       </c>
-      <c r="J15" s="8">
+      <c r="K15" s="8">
         <v>4</v>
-      </c>
-      <c r="K15" s="8">
-        <v>3</v>
       </c>
       <c r="L15" s="8">
         <v>3</v>
       </c>
       <c r="M15" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N15" s="8">
         <v>2</v>
@@ -1501,13 +1535,16 @@
         <v>2</v>
       </c>
       <c r="P15" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>43910</v>
       </c>
@@ -1516,39 +1553,39 @@
         <v>15</v>
       </c>
       <c r="C16" s="8">
+        <v>5</v>
+      </c>
+      <c r="D16" s="8">
         <v>263</v>
       </c>
-      <c r="D16" s="8">
-        <f>C16-C15</f>
+      <c r="E16" s="8">
+        <f>D16-D15</f>
         <v>29</v>
       </c>
-      <c r="E16" s="8">
+      <c r="F16" s="8">
         <v>3</v>
       </c>
-      <c r="F16" s="8">
+      <c r="G16" s="8">
         <v>212</v>
       </c>
-      <c r="G16" s="8">
+      <c r="H16" s="8">
         <v>12</v>
       </c>
-      <c r="H16" s="8">
+      <c r="I16" s="8">
         <v>6</v>
       </c>
-      <c r="I16" s="8">
+      <c r="J16" s="8">
         <v>5</v>
-      </c>
-      <c r="J16" s="8">
-        <v>4</v>
       </c>
       <c r="K16" s="8">
         <v>4</v>
       </c>
       <c r="L16" s="8">
+        <v>4</v>
+      </c>
+      <c r="M16" s="8">
         <v>3</v>
       </c>
-      <c r="M16" s="8">
-        <v>2</v>
-      </c>
       <c r="N16" s="8">
         <v>2</v>
       </c>
@@ -1556,16 +1593,19 @@
         <v>2</v>
       </c>
       <c r="P16" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q16" s="8">
         <v>1</v>
       </c>
       <c r="R16" s="8">
+        <v>1</v>
+      </c>
+      <c r="S16" s="8">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>43911</v>
       </c>
@@ -1574,29 +1614,29 @@
         <v>16</v>
       </c>
       <c r="C17" s="8">
+        <v>6</v>
+      </c>
+      <c r="D17" s="8">
         <v>318</v>
       </c>
-      <c r="D17" s="8">
-        <f>C17-C16</f>
+      <c r="E17" s="8">
+        <f>D17-D16</f>
         <v>55</v>
       </c>
-      <c r="E17" s="8">
+      <c r="F17" s="8">
         <v>5</v>
       </c>
-      <c r="F17" s="8">
+      <c r="G17" s="8">
         <v>241</v>
       </c>
-      <c r="G17" s="8">
+      <c r="H17" s="8">
         <v>14</v>
       </c>
-      <c r="H17" s="8">
+      <c r="I17" s="8">
         <v>8</v>
       </c>
-      <c r="I17" s="8">
+      <c r="J17" s="8">
         <v>6</v>
-      </c>
-      <c r="J17" s="8">
-        <v>4</v>
       </c>
       <c r="K17" s="8">
         <v>4</v>
@@ -1605,25 +1645,28 @@
         <v>4</v>
       </c>
       <c r="M17" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N17" s="8">
+        <v>2</v>
+      </c>
+      <c r="O17" s="8">
         <v>5</v>
       </c>
-      <c r="O17" s="8">
+      <c r="P17" s="8">
         <v>18</v>
       </c>
-      <c r="P17" s="8">
-        <v>1</v>
-      </c>
       <c r="Q17" s="8">
         <v>1</v>
       </c>
       <c r="R17" s="8">
+        <v>1</v>
+      </c>
+      <c r="S17" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>43912</v>
       </c>
@@ -1632,114 +1675,184 @@
         <v>17</v>
       </c>
       <c r="C18" s="8">
+        <v>7</v>
+      </c>
+      <c r="D18" s="8">
         <v>363</v>
       </c>
-      <c r="D18" s="8">
-        <f>C18-C17</f>
+      <c r="E18" s="8">
+        <f>D18-D17</f>
         <v>45</v>
       </c>
-      <c r="E18" s="8">
+      <c r="F18" s="8">
         <v>5</v>
       </c>
-      <c r="F18" s="8">
+      <c r="G18" s="8">
         <v>278</v>
       </c>
-      <c r="G18" s="8">
+      <c r="H18" s="8">
         <v>16</v>
       </c>
-      <c r="H18" s="8">
+      <c r="I18" s="8">
         <v>8</v>
       </c>
-      <c r="I18" s="8">
+      <c r="J18" s="8">
         <v>6</v>
-      </c>
-      <c r="J18" s="8">
-        <v>4</v>
       </c>
       <c r="K18" s="8">
         <v>4</v>
       </c>
       <c r="L18" s="8">
+        <v>4</v>
+      </c>
+      <c r="M18" s="8">
         <v>7</v>
       </c>
-      <c r="M18" s="8">
+      <c r="N18" s="8">
         <v>4</v>
       </c>
-      <c r="N18" s="8">
+      <c r="O18" s="8">
         <v>5</v>
       </c>
-      <c r="O18" s="8">
+      <c r="P18" s="8">
         <v>19</v>
       </c>
-      <c r="P18" s="8">
-        <v>1</v>
-      </c>
       <c r="Q18" s="8">
         <v>1</v>
       </c>
       <c r="R18" s="8">
+        <v>1</v>
+      </c>
+      <c r="S18" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
-        <v>43912</v>
+        <v>43913</v>
       </c>
       <c r="B19" s="8">
-        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C19" s="8">
+        <v>8</v>
+      </c>
+      <c r="D19" s="8">
         <v>395</v>
       </c>
-      <c r="D19" s="8">
-        <f>C19-C18</f>
+      <c r="E19" s="8">
         <v>32</v>
       </c>
-      <c r="E19" s="8">
+      <c r="F19" s="8">
         <v>5</v>
       </c>
-      <c r="F19" s="8">
+      <c r="G19" s="8">
         <v>307</v>
       </c>
-      <c r="G19" s="8">
+      <c r="H19" s="8">
         <v>16</v>
-      </c>
-      <c r="H19" s="8">
-        <v>8</v>
       </c>
       <c r="I19" s="8">
         <v>8</v>
       </c>
       <c r="J19" s="8">
+        <v>8</v>
+      </c>
+      <c r="K19" s="8">
         <v>6</v>
       </c>
-      <c r="K19" s="8">
+      <c r="L19" s="8">
         <v>4</v>
       </c>
-      <c r="L19" s="8">
+      <c r="M19" s="8">
         <v>7</v>
       </c>
-      <c r="M19" s="8">
-        <v>2</v>
-      </c>
       <c r="N19" s="8">
+        <v>2</v>
+      </c>
+      <c r="O19" s="8">
         <v>4</v>
       </c>
-      <c r="O19" s="8">
+      <c r="P19" s="8">
         <v>19</v>
       </c>
-      <c r="P19" s="8">
-        <v>2</v>
-      </c>
       <c r="Q19" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R19" s="8">
+        <v>1</v>
+      </c>
+      <c r="S19" s="8">
         <v>10</v>
       </c>
-      <c r="AA19">
-        <v>1</v>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>43914</v>
+      </c>
+      <c r="B20" s="8">
+        <v>19</v>
+      </c>
+      <c r="C20" s="8">
+        <v>9</v>
+      </c>
+      <c r="D20" s="8">
+        <v>416</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" ref="E19:E20" si="2">D20-D19</f>
+        <v>21</v>
+      </c>
+      <c r="F20" s="8">
+        <v>5</v>
+      </c>
+      <c r="G20" s="8">
+        <v>322</v>
+      </c>
+      <c r="H20" s="8">
+        <v>16</v>
+      </c>
+      <c r="I20" s="8">
+        <v>8</v>
+      </c>
+      <c r="J20" s="8">
+        <v>8</v>
+      </c>
+      <c r="K20" s="8">
+        <v>6</v>
+      </c>
+      <c r="L20" s="8">
+        <v>4</v>
+      </c>
+      <c r="M20" s="8">
+        <v>9</v>
+      </c>
+      <c r="N20" s="8">
+        <v>2</v>
+      </c>
+      <c r="O20" s="8">
+        <v>5</v>
+      </c>
+      <c r="P20" s="8">
+        <v>19</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>2</v>
+      </c>
+      <c r="R20" s="8">
+        <v>1</v>
+      </c>
+      <c r="S20" s="8">
+        <v>10</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1748,6 +1861,100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85C99E3-EBDD-4539-8A6F-F0A7A14DC87E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D3763C-0359-41B9-A88E-D43678C96FA1}">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="10">
+        <v>43913</v>
+      </c>
+      <c r="B1" s="8">
+        <v>18</v>
+      </c>
+      <c r="C1" s="8">
+        <v>8</v>
+      </c>
+      <c r="D1" s="8">
+        <v>395</v>
+      </c>
+      <c r="E1" s="8">
+        <v>32</v>
+      </c>
+      <c r="F1" s="8">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8">
+        <v>307</v>
+      </c>
+      <c r="H1" s="8">
+        <v>16</v>
+      </c>
+      <c r="I1" s="8">
+        <v>8</v>
+      </c>
+      <c r="J1" s="8">
+        <v>8</v>
+      </c>
+      <c r="K1" s="8">
+        <v>6</v>
+      </c>
+      <c r="L1" s="8">
+        <v>4</v>
+      </c>
+      <c r="M1" s="8">
+        <v>7</v>
+      </c>
+      <c r="N1" s="8">
+        <v>2</v>
+      </c>
+      <c r="O1" s="8">
+        <v>4</v>
+      </c>
+      <c r="P1" s="8">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="8">
+        <v>2</v>
+      </c>
+      <c r="R1" s="8">
+        <v>1</v>
+      </c>
+      <c r="S1" s="8">
+        <v>10</v>
+      </c>
+      <c r="AB1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49973FC-C21B-419D-86C5-7EE8496B9B44}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1787,11 +1994,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15ADEF6E-6768-4EE4-A06F-16116EB8E717}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -1800,7 +2007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA75DE2-DFBF-4DD1-886E-7BF3BF81DB3E}">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -2101,7 +2308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D305DDB7-21EF-4064-9B3A-06591E83BC3A}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
@@ -2633,7 +2840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A4C348-BB07-4639-A7E1-78743117ECCB}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -2775,7 +2982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D2EFCE-C058-4F04-B471-51945290F2EA}">
   <dimension ref="A1:D7"/>
   <sheetViews>

</xml_diff>